<commit_message>
added files for compProf simulation
</commit_message>
<xml_diff>
--- a/data/codebook.xlsx
+++ b/data/codebook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmaj\Documents\Poor comprehenders SDAI\ALSPAC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmaj\Documents\Poor comprehenders SDAI\WP1 - Identification\ESRC_EJ_WP1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4FAA6B-584C-407A-A6AC-9A55EE5C8A3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8B85DD-D096-4927-BCBD-59F0A40E6AB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31650" yWindow="2175" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="2" r:id="rId1"/>
@@ -11664,8 +11664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1063"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A253" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D282" sqref="D282"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K124" sqref="K124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16394,7 +16394,7 @@
       </c>
       <c r="K143" s="2"/>
       <c r="L143" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:12" x14ac:dyDescent="0.25">
@@ -16430,7 +16430,7 @@
       </c>
       <c r="K144" s="2"/>
       <c r="L144" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:12" x14ac:dyDescent="0.25">
@@ -16466,7 +16466,7 @@
       </c>
       <c r="K145" s="2"/>
       <c r="L145" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:12" x14ac:dyDescent="0.25">
@@ -16502,7 +16502,7 @@
       </c>
       <c r="K146" s="2"/>
       <c r="L146" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
@@ -16538,7 +16538,7 @@
       </c>
       <c r="K147" s="2"/>
       <c r="L147" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
@@ -16970,7 +16970,7 @@
       </c>
       <c r="K159" s="2"/>
       <c r="L159" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:12" x14ac:dyDescent="0.25">
@@ -21326,7 +21326,7 @@
       </c>
       <c r="K280" s="2"/>
       <c r="L280" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="281" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>